<commit_message>
Fixed analysis of IBM through adding language manually
</commit_message>
<xml_diff>
--- a/Datasets/Analysed Dataset (no calc)/IBM/Excel (readable)/Uber_Result.xlsx
+++ b/Datasets/Analysed Dataset (no calc)/IBM/Excel (readable)/Uber_Result.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QuangDaoVuNgoc\github\bachelorthesis\Datasets\Analysed Dataset (no calc)\IBM\Excel (readable)\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{048EE2C1-511C-421D-9B60-45D42EE7F206}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F79353C-EF9A-4FFC-A555-5C08BA421F8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="28110" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,8 +16,8 @@
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Uber_Result" localSheetId="0">Tabelle1!$C$1:$D$936</definedName>
-    <definedName name="Vader_Analysed_Uber_Ride_Reviews" localSheetId="0">Tabelle1!$A$1:$B$936</definedName>
+    <definedName name="Uber_Result" localSheetId="0">Tabelle1!$C$1:$D$937</definedName>
+    <definedName name="Vader_Analysed_Uber_Ride_Reviews" localSheetId="0">Tabelle1!$A$1:$B$937</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -55,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1871" uniqueCount="1858">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1873" uniqueCount="1860">
   <si>
     <t>Polarity</t>
   </si>
@@ -5629,6 +5629,12 @@
   </si>
   <si>
     <t>Polarity_result</t>
+  </si>
+  <si>
+    <t>uber crooked</t>
+  </si>
+  <si>
+    <t>-0.87784</t>
   </si>
 </sst>
 </file>
@@ -5684,11 +5690,11 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Uber_Result" connectionId="1" xr16:uid="{59614B44-6B4D-4428-ADC8-0DDED0E8C730}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Vader_Analysed_Uber_Ride_Reviews" connectionId="2" xr16:uid="{5A50E92B-E150-44E0-A9FA-AF734AA2CF4E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Vader_Analysed_Uber_Ride_Reviews" connectionId="2" xr16:uid="{5A50E92B-E150-44E0-A9FA-AF734AA2CF4E}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Uber_Result" connectionId="1" xr16:uid="{59614B44-6B4D-4428-ADC8-0DDED0E8C730}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5954,10 +5960,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D936"/>
+  <dimension ref="A1:D937"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="A715" workbookViewId="0">
+      <selection activeCell="E744" sqref="E744"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16374,10 +16380,10 @@
         <v>-1</v>
       </c>
       <c r="B744" t="s">
-        <v>742</v>
+        <v>1858</v>
       </c>
       <c r="C744" t="s">
-        <v>1665</v>
+        <v>1859</v>
       </c>
       <c r="D744">
         <v>-1</v>
@@ -16385,13 +16391,13 @@
     </row>
     <row r="745" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A745">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B745" t="s">
-        <v>743</v>
+        <v>742</v>
       </c>
       <c r="C745" t="s">
-        <v>1666</v>
+        <v>1665</v>
       </c>
       <c r="D745">
         <v>-1</v>
@@ -16399,13 +16405,13 @@
     </row>
     <row r="746" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A746">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B746" t="s">
-        <v>744</v>
+        <v>743</v>
       </c>
       <c r="C746" t="s">
-        <v>1667</v>
+        <v>1666</v>
       </c>
       <c r="D746">
         <v>-1</v>
@@ -16416,10 +16422,10 @@
         <v>-1</v>
       </c>
       <c r="B747" t="s">
-        <v>745</v>
+        <v>744</v>
       </c>
       <c r="C747" t="s">
-        <v>1668</v>
+        <v>1667</v>
       </c>
       <c r="D747">
         <v>-1</v>
@@ -16430,10 +16436,10 @@
         <v>-1</v>
       </c>
       <c r="B748" t="s">
-        <v>746</v>
+        <v>745</v>
       </c>
       <c r="C748" t="s">
-        <v>1669</v>
+        <v>1668</v>
       </c>
       <c r="D748">
         <v>-1</v>
@@ -16441,16 +16447,16 @@
     </row>
     <row r="749" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A749">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B749" t="s">
-        <v>747</v>
+        <v>746</v>
       </c>
       <c r="C749" t="s">
-        <v>1670</v>
+        <v>1669</v>
       </c>
       <c r="D749">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="750" spans="1:4" x14ac:dyDescent="0.25">
@@ -16458,10 +16464,10 @@
         <v>1</v>
       </c>
       <c r="B750" t="s">
-        <v>748</v>
+        <v>747</v>
       </c>
       <c r="C750" t="s">
-        <v>1671</v>
+        <v>1670</v>
       </c>
       <c r="D750">
         <v>1</v>
@@ -16469,16 +16475,16 @@
     </row>
     <row r="751" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A751">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B751" t="s">
-        <v>749</v>
+        <v>748</v>
       </c>
       <c r="C751" t="s">
-        <v>1672</v>
+        <v>1671</v>
       </c>
       <c r="D751">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="752" spans="1:4" x14ac:dyDescent="0.25">
@@ -16486,10 +16492,10 @@
         <v>-1</v>
       </c>
       <c r="B752" t="s">
-        <v>750</v>
+        <v>749</v>
       </c>
       <c r="C752" t="s">
-        <v>1673</v>
+        <v>1672</v>
       </c>
       <c r="D752">
         <v>-1</v>
@@ -16500,10 +16506,10 @@
         <v>-1</v>
       </c>
       <c r="B753" t="s">
-        <v>751</v>
+        <v>750</v>
       </c>
       <c r="C753" t="s">
-        <v>1674</v>
+        <v>1673</v>
       </c>
       <c r="D753">
         <v>-1</v>
@@ -16514,10 +16520,10 @@
         <v>-1</v>
       </c>
       <c r="B754" t="s">
-        <v>752</v>
+        <v>751</v>
       </c>
       <c r="C754" t="s">
-        <v>1675</v>
+        <v>1674</v>
       </c>
       <c r="D754">
         <v>-1</v>
@@ -16528,10 +16534,10 @@
         <v>-1</v>
       </c>
       <c r="B755" t="s">
-        <v>753</v>
+        <v>752</v>
       </c>
       <c r="C755" t="s">
-        <v>1676</v>
+        <v>1675</v>
       </c>
       <c r="D755">
         <v>-1</v>
@@ -16542,10 +16548,10 @@
         <v>-1</v>
       </c>
       <c r="B756" t="s">
-        <v>754</v>
+        <v>753</v>
       </c>
       <c r="C756" t="s">
-        <v>1677</v>
+        <v>1676</v>
       </c>
       <c r="D756">
         <v>-1</v>
@@ -16556,10 +16562,10 @@
         <v>-1</v>
       </c>
       <c r="B757" t="s">
-        <v>755</v>
+        <v>754</v>
       </c>
       <c r="C757" t="s">
-        <v>1678</v>
+        <v>1677</v>
       </c>
       <c r="D757">
         <v>-1</v>
@@ -16570,10 +16576,10 @@
         <v>-1</v>
       </c>
       <c r="B758" t="s">
-        <v>756</v>
+        <v>755</v>
       </c>
       <c r="C758" t="s">
-        <v>1679</v>
+        <v>1678</v>
       </c>
       <c r="D758">
         <v>-1</v>
@@ -16584,10 +16590,10 @@
         <v>-1</v>
       </c>
       <c r="B759" t="s">
-        <v>757</v>
+        <v>756</v>
       </c>
       <c r="C759" t="s">
-        <v>1680</v>
+        <v>1679</v>
       </c>
       <c r="D759">
         <v>-1</v>
@@ -16595,13 +16601,13 @@
     </row>
     <row r="760" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A760">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B760" t="s">
-        <v>758</v>
+        <v>757</v>
       </c>
       <c r="C760" t="s">
-        <v>1681</v>
+        <v>1680</v>
       </c>
       <c r="D760">
         <v>-1</v>
@@ -16609,13 +16615,13 @@
     </row>
     <row r="761" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A761">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B761" t="s">
-        <v>759</v>
+        <v>758</v>
       </c>
       <c r="C761" t="s">
-        <v>1682</v>
+        <v>1681</v>
       </c>
       <c r="D761">
         <v>-1</v>
@@ -16626,10 +16632,10 @@
         <v>-1</v>
       </c>
       <c r="B762" t="s">
-        <v>760</v>
+        <v>759</v>
       </c>
       <c r="C762" t="s">
-        <v>1311</v>
+        <v>1682</v>
       </c>
       <c r="D762">
         <v>-1</v>
@@ -16640,10 +16646,10 @@
         <v>-1</v>
       </c>
       <c r="B763" t="s">
-        <v>761</v>
+        <v>760</v>
       </c>
       <c r="C763" t="s">
-        <v>1683</v>
+        <v>1311</v>
       </c>
       <c r="D763">
         <v>-1</v>
@@ -16654,10 +16660,10 @@
         <v>-1</v>
       </c>
       <c r="B764" t="s">
-        <v>762</v>
+        <v>761</v>
       </c>
       <c r="C764" t="s">
-        <v>1684</v>
+        <v>1683</v>
       </c>
       <c r="D764">
         <v>-1</v>
@@ -16668,13 +16674,13 @@
         <v>-1</v>
       </c>
       <c r="B765" t="s">
-        <v>763</v>
+        <v>762</v>
       </c>
       <c r="C765" t="s">
-        <v>1685</v>
+        <v>1684</v>
       </c>
       <c r="D765">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="766" spans="1:4" x14ac:dyDescent="0.25">
@@ -16682,13 +16688,13 @@
         <v>-1</v>
       </c>
       <c r="B766" t="s">
-        <v>764</v>
+        <v>763</v>
       </c>
       <c r="C766" t="s">
-        <v>1686</v>
+        <v>1685</v>
       </c>
       <c r="D766">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="767" spans="1:4" x14ac:dyDescent="0.25">
@@ -16696,10 +16702,10 @@
         <v>-1</v>
       </c>
       <c r="B767" t="s">
-        <v>765</v>
+        <v>764</v>
       </c>
       <c r="C767" t="s">
-        <v>1687</v>
+        <v>1686</v>
       </c>
       <c r="D767">
         <v>-1</v>
@@ -16710,10 +16716,10 @@
         <v>-1</v>
       </c>
       <c r="B768" t="s">
-        <v>766</v>
+        <v>765</v>
       </c>
       <c r="C768" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
       <c r="D768">
         <v>-1</v>
@@ -16721,16 +16727,16 @@
     </row>
     <row r="769" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A769">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B769" t="s">
-        <v>767</v>
+        <v>766</v>
       </c>
       <c r="C769" t="s">
-        <v>1689</v>
+        <v>1688</v>
       </c>
       <c r="D769">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="770" spans="1:4" x14ac:dyDescent="0.25">
@@ -16738,24 +16744,24 @@
         <v>1</v>
       </c>
       <c r="B770" t="s">
-        <v>768</v>
+        <v>767</v>
       </c>
       <c r="C770" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
       <c r="D770">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="771" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A771">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B771" t="s">
-        <v>769</v>
+        <v>768</v>
       </c>
       <c r="C771" t="s">
-        <v>1691</v>
+        <v>1690</v>
       </c>
       <c r="D771">
         <v>-1</v>
@@ -16766,10 +16772,10 @@
         <v>-1</v>
       </c>
       <c r="B772" t="s">
-        <v>770</v>
+        <v>769</v>
       </c>
       <c r="C772" t="s">
-        <v>1692</v>
+        <v>1691</v>
       </c>
       <c r="D772">
         <v>-1</v>
@@ -16780,10 +16786,10 @@
         <v>-1</v>
       </c>
       <c r="B773" t="s">
-        <v>771</v>
+        <v>770</v>
       </c>
       <c r="C773" t="s">
-        <v>1693</v>
+        <v>1692</v>
       </c>
       <c r="D773">
         <v>-1</v>
@@ -16794,10 +16800,10 @@
         <v>-1</v>
       </c>
       <c r="B774" t="s">
-        <v>772</v>
+        <v>771</v>
       </c>
       <c r="C774" t="s">
-        <v>1694</v>
+        <v>1693</v>
       </c>
       <c r="D774">
         <v>-1</v>
@@ -16808,10 +16814,10 @@
         <v>-1</v>
       </c>
       <c r="B775" t="s">
-        <v>773</v>
+        <v>772</v>
       </c>
       <c r="C775" t="s">
-        <v>1695</v>
+        <v>1694</v>
       </c>
       <c r="D775">
         <v>-1</v>
@@ -16822,10 +16828,10 @@
         <v>-1</v>
       </c>
       <c r="B776" t="s">
-        <v>774</v>
+        <v>773</v>
       </c>
       <c r="C776" t="s">
-        <v>1696</v>
+        <v>1695</v>
       </c>
       <c r="D776">
         <v>-1</v>
@@ -16836,10 +16842,10 @@
         <v>-1</v>
       </c>
       <c r="B777" t="s">
-        <v>775</v>
+        <v>774</v>
       </c>
       <c r="C777" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
       <c r="D777">
         <v>-1</v>
@@ -16850,10 +16856,10 @@
         <v>-1</v>
       </c>
       <c r="B778" t="s">
-        <v>776</v>
+        <v>775</v>
       </c>
       <c r="C778" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
       <c r="D778">
         <v>-1</v>
@@ -16864,10 +16870,10 @@
         <v>-1</v>
       </c>
       <c r="B779" t="s">
-        <v>777</v>
+        <v>776</v>
       </c>
       <c r="C779" t="s">
-        <v>1699</v>
+        <v>1698</v>
       </c>
       <c r="D779">
         <v>-1</v>
@@ -16875,30 +16881,30 @@
     </row>
     <row r="780" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A780">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B780" t="s">
-        <v>778</v>
+        <v>777</v>
       </c>
       <c r="C780" t="s">
-        <v>1700</v>
+        <v>1699</v>
       </c>
       <c r="D780">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="781" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A781">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B781" t="s">
-        <v>779</v>
+        <v>778</v>
       </c>
       <c r="C781" t="s">
-        <v>1701</v>
+        <v>1700</v>
       </c>
       <c r="D781">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="782" spans="1:4" x14ac:dyDescent="0.25">
@@ -16906,10 +16912,10 @@
         <v>-1</v>
       </c>
       <c r="B782" t="s">
-        <v>780</v>
+        <v>779</v>
       </c>
       <c r="C782" t="s">
-        <v>1702</v>
+        <v>1701</v>
       </c>
       <c r="D782">
         <v>-1</v>
@@ -16920,10 +16926,10 @@
         <v>-1</v>
       </c>
       <c r="B783" t="s">
-        <v>781</v>
+        <v>780</v>
       </c>
       <c r="C783" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
       <c r="D783">
         <v>-1</v>
@@ -16934,10 +16940,10 @@
         <v>-1</v>
       </c>
       <c r="B784" t="s">
-        <v>782</v>
+        <v>781</v>
       </c>
       <c r="C784" t="s">
-        <v>1704</v>
+        <v>1703</v>
       </c>
       <c r="D784">
         <v>-1</v>
@@ -16948,10 +16954,10 @@
         <v>-1</v>
       </c>
       <c r="B785" t="s">
-        <v>783</v>
+        <v>782</v>
       </c>
       <c r="C785" t="s">
-        <v>1705</v>
+        <v>1704</v>
       </c>
       <c r="D785">
         <v>-1</v>
@@ -16962,10 +16968,10 @@
         <v>-1</v>
       </c>
       <c r="B786" t="s">
-        <v>784</v>
+        <v>783</v>
       </c>
       <c r="C786" t="s">
-        <v>1706</v>
+        <v>1705</v>
       </c>
       <c r="D786">
         <v>-1</v>
@@ -16976,10 +16982,10 @@
         <v>-1</v>
       </c>
       <c r="B787" t="s">
-        <v>785</v>
+        <v>784</v>
       </c>
       <c r="C787" t="s">
-        <v>1707</v>
+        <v>1706</v>
       </c>
       <c r="D787">
         <v>-1</v>
@@ -16990,10 +16996,10 @@
         <v>-1</v>
       </c>
       <c r="B788" t="s">
-        <v>786</v>
+        <v>785</v>
       </c>
       <c r="C788" t="s">
-        <v>1708</v>
+        <v>1707</v>
       </c>
       <c r="D788">
         <v>-1</v>
@@ -17004,10 +17010,10 @@
         <v>-1</v>
       </c>
       <c r="B789" t="s">
-        <v>787</v>
+        <v>786</v>
       </c>
       <c r="C789" t="s">
-        <v>1709</v>
+        <v>1708</v>
       </c>
       <c r="D789">
         <v>-1</v>
@@ -17018,10 +17024,10 @@
         <v>-1</v>
       </c>
       <c r="B790" t="s">
-        <v>788</v>
+        <v>787</v>
       </c>
       <c r="C790" t="s">
-        <v>1710</v>
+        <v>1709</v>
       </c>
       <c r="D790">
         <v>-1</v>
@@ -17032,10 +17038,10 @@
         <v>-1</v>
       </c>
       <c r="B791" t="s">
-        <v>789</v>
+        <v>788</v>
       </c>
       <c r="C791" t="s">
-        <v>1711</v>
+        <v>1710</v>
       </c>
       <c r="D791">
         <v>-1</v>
@@ -17046,10 +17052,10 @@
         <v>-1</v>
       </c>
       <c r="B792" t="s">
-        <v>790</v>
+        <v>789</v>
       </c>
       <c r="C792" t="s">
-        <v>1712</v>
+        <v>1711</v>
       </c>
       <c r="D792">
         <v>-1</v>
@@ -17060,10 +17066,10 @@
         <v>-1</v>
       </c>
       <c r="B793" t="s">
-        <v>791</v>
+        <v>790</v>
       </c>
       <c r="C793" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
       <c r="D793">
         <v>-1</v>
@@ -17074,10 +17080,10 @@
         <v>-1</v>
       </c>
       <c r="B794" t="s">
-        <v>792</v>
+        <v>791</v>
       </c>
       <c r="C794" t="s">
-        <v>1714</v>
+        <v>1713</v>
       </c>
       <c r="D794">
         <v>-1</v>
@@ -17088,10 +17094,10 @@
         <v>-1</v>
       </c>
       <c r="B795" t="s">
-        <v>793</v>
+        <v>792</v>
       </c>
       <c r="C795" t="s">
-        <v>1715</v>
+        <v>1714</v>
       </c>
       <c r="D795">
         <v>-1</v>
@@ -17102,10 +17108,10 @@
         <v>-1</v>
       </c>
       <c r="B796" t="s">
-        <v>794</v>
+        <v>793</v>
       </c>
       <c r="C796" t="s">
-        <v>1716</v>
+        <v>1715</v>
       </c>
       <c r="D796">
         <v>-1</v>
@@ -17116,10 +17122,10 @@
         <v>-1</v>
       </c>
       <c r="B797" t="s">
-        <v>795</v>
+        <v>794</v>
       </c>
       <c r="C797" t="s">
-        <v>1717</v>
+        <v>1716</v>
       </c>
       <c r="D797">
         <v>-1</v>
@@ -17127,30 +17133,30 @@
     </row>
     <row r="798" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A798">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B798" t="s">
-        <v>796</v>
+        <v>795</v>
       </c>
       <c r="C798" t="s">
-        <v>1718</v>
+        <v>1717</v>
       </c>
       <c r="D798">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="799" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A799">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B799" t="s">
-        <v>797</v>
+        <v>796</v>
       </c>
       <c r="C799" t="s">
-        <v>1719</v>
+        <v>1718</v>
       </c>
       <c r="D799">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="800" spans="1:4" x14ac:dyDescent="0.25">
@@ -17158,10 +17164,10 @@
         <v>-1</v>
       </c>
       <c r="B800" t="s">
-        <v>798</v>
+        <v>797</v>
       </c>
       <c r="C800" t="s">
-        <v>1720</v>
+        <v>1719</v>
       </c>
       <c r="D800">
         <v>-1</v>
@@ -17172,10 +17178,10 @@
         <v>-1</v>
       </c>
       <c r="B801" t="s">
-        <v>799</v>
+        <v>798</v>
       </c>
       <c r="C801" t="s">
-        <v>1721</v>
+        <v>1720</v>
       </c>
       <c r="D801">
         <v>-1</v>
@@ -17186,10 +17192,10 @@
         <v>-1</v>
       </c>
       <c r="B802" t="s">
-        <v>800</v>
+        <v>799</v>
       </c>
       <c r="C802" t="s">
-        <v>1722</v>
+        <v>1721</v>
       </c>
       <c r="D802">
         <v>-1</v>
@@ -17200,10 +17206,10 @@
         <v>-1</v>
       </c>
       <c r="B803" t="s">
-        <v>801</v>
+        <v>800</v>
       </c>
       <c r="C803" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
       <c r="D803">
         <v>-1</v>
@@ -17214,10 +17220,10 @@
         <v>-1</v>
       </c>
       <c r="B804" t="s">
-        <v>802</v>
+        <v>801</v>
       </c>
       <c r="C804" t="s">
-        <v>1724</v>
+        <v>1723</v>
       </c>
       <c r="D804">
         <v>-1</v>
@@ -17228,10 +17234,10 @@
         <v>-1</v>
       </c>
       <c r="B805" t="s">
-        <v>803</v>
+        <v>802</v>
       </c>
       <c r="C805" t="s">
-        <v>1725</v>
+        <v>1724</v>
       </c>
       <c r="D805">
         <v>-1</v>
@@ -17239,30 +17245,30 @@
     </row>
     <row r="806" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A806">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B806" t="s">
-        <v>804</v>
+        <v>803</v>
       </c>
       <c r="C806" t="s">
-        <v>1726</v>
+        <v>1725</v>
       </c>
       <c r="D806">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="807" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A807">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B807" t="s">
-        <v>805</v>
+        <v>804</v>
       </c>
       <c r="C807" t="s">
-        <v>1727</v>
+        <v>1726</v>
       </c>
       <c r="D807">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="808" spans="1:4" x14ac:dyDescent="0.25">
@@ -17270,10 +17276,10 @@
         <v>-1</v>
       </c>
       <c r="B808" t="s">
-        <v>806</v>
+        <v>805</v>
       </c>
       <c r="C808" t="s">
-        <v>1728</v>
+        <v>1727</v>
       </c>
       <c r="D808">
         <v>-1</v>
@@ -17284,10 +17290,10 @@
         <v>-1</v>
       </c>
       <c r="B809" t="s">
-        <v>807</v>
+        <v>806</v>
       </c>
       <c r="C809" t="s">
-        <v>1729</v>
+        <v>1728</v>
       </c>
       <c r="D809">
         <v>-1</v>
@@ -17298,10 +17304,10 @@
         <v>-1</v>
       </c>
       <c r="B810" t="s">
-        <v>808</v>
+        <v>807</v>
       </c>
       <c r="C810" t="s">
-        <v>1730</v>
+        <v>1729</v>
       </c>
       <c r="D810">
         <v>-1</v>
@@ -17312,10 +17318,10 @@
         <v>-1</v>
       </c>
       <c r="B811" t="s">
-        <v>809</v>
+        <v>808</v>
       </c>
       <c r="C811" t="s">
-        <v>1731</v>
+        <v>1730</v>
       </c>
       <c r="D811">
         <v>-1</v>
@@ -17326,10 +17332,10 @@
         <v>-1</v>
       </c>
       <c r="B812" t="s">
-        <v>810</v>
+        <v>809</v>
       </c>
       <c r="C812" t="s">
-        <v>1732</v>
+        <v>1731</v>
       </c>
       <c r="D812">
         <v>-1</v>
@@ -17340,10 +17346,10 @@
         <v>-1</v>
       </c>
       <c r="B813" t="s">
-        <v>811</v>
+        <v>810</v>
       </c>
       <c r="C813" t="s">
-        <v>1733</v>
+        <v>1732</v>
       </c>
       <c r="D813">
         <v>-1</v>
@@ -17354,10 +17360,10 @@
         <v>-1</v>
       </c>
       <c r="B814" t="s">
-        <v>812</v>
+        <v>811</v>
       </c>
       <c r="C814" t="s">
-        <v>1734</v>
+        <v>1733</v>
       </c>
       <c r="D814">
         <v>-1</v>
@@ -17368,10 +17374,10 @@
         <v>-1</v>
       </c>
       <c r="B815" t="s">
-        <v>813</v>
+        <v>812</v>
       </c>
       <c r="C815" t="s">
-        <v>1735</v>
+        <v>1734</v>
       </c>
       <c r="D815">
         <v>-1</v>
@@ -17382,10 +17388,10 @@
         <v>-1</v>
       </c>
       <c r="B816" t="s">
-        <v>814</v>
+        <v>813</v>
       </c>
       <c r="C816" t="s">
-        <v>1736</v>
+        <v>1735</v>
       </c>
       <c r="D816">
         <v>-1</v>
@@ -17396,10 +17402,10 @@
         <v>-1</v>
       </c>
       <c r="B817" t="s">
-        <v>815</v>
+        <v>814</v>
       </c>
       <c r="C817" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
       <c r="D817">
         <v>-1</v>
@@ -17410,10 +17416,10 @@
         <v>-1</v>
       </c>
       <c r="B818" t="s">
-        <v>816</v>
+        <v>815</v>
       </c>
       <c r="C818" t="s">
-        <v>1738</v>
+        <v>1737</v>
       </c>
       <c r="D818">
         <v>-1</v>
@@ -17424,10 +17430,10 @@
         <v>-1</v>
       </c>
       <c r="B819" t="s">
-        <v>817</v>
+        <v>816</v>
       </c>
       <c r="C819" t="s">
-        <v>1739</v>
+        <v>1738</v>
       </c>
       <c r="D819">
         <v>-1</v>
@@ -17438,10 +17444,10 @@
         <v>-1</v>
       </c>
       <c r="B820" t="s">
-        <v>818</v>
+        <v>817</v>
       </c>
       <c r="C820" t="s">
-        <v>1740</v>
+        <v>1739</v>
       </c>
       <c r="D820">
         <v>-1</v>
@@ -17452,10 +17458,10 @@
         <v>-1</v>
       </c>
       <c r="B821" t="s">
-        <v>819</v>
+        <v>818</v>
       </c>
       <c r="C821" t="s">
-        <v>1741</v>
+        <v>1740</v>
       </c>
       <c r="D821">
         <v>-1</v>
@@ -17466,10 +17472,10 @@
         <v>-1</v>
       </c>
       <c r="B822" t="s">
-        <v>820</v>
+        <v>819</v>
       </c>
       <c r="C822" t="s">
-        <v>1742</v>
+        <v>1741</v>
       </c>
       <c r="D822">
         <v>-1</v>
@@ -17480,10 +17486,10 @@
         <v>-1</v>
       </c>
       <c r="B823" t="s">
-        <v>821</v>
+        <v>820</v>
       </c>
       <c r="C823" t="s">
-        <v>1743</v>
+        <v>1742</v>
       </c>
       <c r="D823">
         <v>-1</v>
@@ -17494,10 +17500,10 @@
         <v>-1</v>
       </c>
       <c r="B824" t="s">
-        <v>822</v>
+        <v>821</v>
       </c>
       <c r="C824" t="s">
-        <v>1744</v>
+        <v>1743</v>
       </c>
       <c r="D824">
         <v>-1</v>
@@ -17508,10 +17514,10 @@
         <v>-1</v>
       </c>
       <c r="B825" t="s">
-        <v>823</v>
+        <v>822</v>
       </c>
       <c r="C825" t="s">
-        <v>1745</v>
+        <v>1744</v>
       </c>
       <c r="D825">
         <v>-1</v>
@@ -17522,10 +17528,10 @@
         <v>-1</v>
       </c>
       <c r="B826" t="s">
-        <v>824</v>
+        <v>823</v>
       </c>
       <c r="C826" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
       <c r="D826">
         <v>-1</v>
@@ -17536,10 +17542,10 @@
         <v>-1</v>
       </c>
       <c r="B827" t="s">
-        <v>825</v>
+        <v>824</v>
       </c>
       <c r="C827" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
       <c r="D827">
         <v>-1</v>
@@ -17550,13 +17556,13 @@
         <v>-1</v>
       </c>
       <c r="B828" t="s">
-        <v>826</v>
+        <v>825</v>
       </c>
       <c r="C828" t="s">
-        <v>1748</v>
+        <v>1747</v>
       </c>
       <c r="D828">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="829" spans="1:4" x14ac:dyDescent="0.25">
@@ -17564,10 +17570,10 @@
         <v>-1</v>
       </c>
       <c r="B829" t="s">
-        <v>827</v>
+        <v>826</v>
       </c>
       <c r="C829" t="s">
-        <v>1749</v>
+        <v>1748</v>
       </c>
       <c r="D829">
         <v>1</v>
@@ -17578,13 +17584,13 @@
         <v>-1</v>
       </c>
       <c r="B830" t="s">
-        <v>828</v>
+        <v>827</v>
       </c>
       <c r="C830" t="s">
-        <v>1750</v>
+        <v>1749</v>
       </c>
       <c r="D830">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="831" spans="1:4" x14ac:dyDescent="0.25">
@@ -17592,10 +17598,10 @@
         <v>-1</v>
       </c>
       <c r="B831" t="s">
-        <v>829</v>
+        <v>828</v>
       </c>
       <c r="C831" t="s">
-        <v>1751</v>
+        <v>1750</v>
       </c>
       <c r="D831">
         <v>-1</v>
@@ -17606,10 +17612,10 @@
         <v>-1</v>
       </c>
       <c r="B832" t="s">
-        <v>830</v>
+        <v>829</v>
       </c>
       <c r="C832" t="s">
-        <v>1752</v>
+        <v>1751</v>
       </c>
       <c r="D832">
         <v>-1</v>
@@ -17617,13 +17623,13 @@
     </row>
     <row r="833" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A833">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B833" t="s">
-        <v>831</v>
+        <v>830</v>
       </c>
       <c r="C833" t="s">
-        <v>1753</v>
+        <v>1752</v>
       </c>
       <c r="D833">
         <v>-1</v>
@@ -17631,13 +17637,13 @@
     </row>
     <row r="834" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A834">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B834" t="s">
-        <v>832</v>
+        <v>831</v>
       </c>
       <c r="C834" t="s">
-        <v>1754</v>
+        <v>1753</v>
       </c>
       <c r="D834">
         <v>-1</v>
@@ -17648,10 +17654,10 @@
         <v>-1</v>
       </c>
       <c r="B835" t="s">
-        <v>833</v>
+        <v>832</v>
       </c>
       <c r="C835" t="s">
-        <v>1755</v>
+        <v>1754</v>
       </c>
       <c r="D835">
         <v>-1</v>
@@ -17662,10 +17668,10 @@
         <v>-1</v>
       </c>
       <c r="B836" t="s">
-        <v>834</v>
+        <v>833</v>
       </c>
       <c r="C836" t="s">
-        <v>1756</v>
+        <v>1755</v>
       </c>
       <c r="D836">
         <v>-1</v>
@@ -17676,13 +17682,13 @@
         <v>-1</v>
       </c>
       <c r="B837" t="s">
-        <v>835</v>
+        <v>834</v>
       </c>
       <c r="C837" t="s">
-        <v>1757</v>
+        <v>1756</v>
       </c>
       <c r="D837">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="838" spans="1:4" x14ac:dyDescent="0.25">
@@ -17690,13 +17696,13 @@
         <v>-1</v>
       </c>
       <c r="B838" t="s">
-        <v>836</v>
+        <v>835</v>
       </c>
       <c r="C838" t="s">
-        <v>1758</v>
+        <v>1757</v>
       </c>
       <c r="D838">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="839" spans="1:4" x14ac:dyDescent="0.25">
@@ -17704,10 +17710,10 @@
         <v>-1</v>
       </c>
       <c r="B839" t="s">
-        <v>837</v>
+        <v>836</v>
       </c>
       <c r="C839" t="s">
-        <v>1759</v>
+        <v>1758</v>
       </c>
       <c r="D839">
         <v>-1</v>
@@ -17715,30 +17721,30 @@
     </row>
     <row r="840" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A840">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B840" t="s">
-        <v>838</v>
+        <v>837</v>
       </c>
       <c r="C840" t="s">
-        <v>1760</v>
+        <v>1759</v>
       </c>
       <c r="D840">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="841" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A841">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B841" t="s">
-        <v>839</v>
+        <v>838</v>
       </c>
       <c r="C841" t="s">
-        <v>1761</v>
+        <v>1760</v>
       </c>
       <c r="D841">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="842" spans="1:4" x14ac:dyDescent="0.25">
@@ -17746,10 +17752,10 @@
         <v>-1</v>
       </c>
       <c r="B842" t="s">
-        <v>840</v>
+        <v>839</v>
       </c>
       <c r="C842" t="s">
-        <v>1762</v>
+        <v>1761</v>
       </c>
       <c r="D842">
         <v>-1</v>
@@ -17760,10 +17766,10 @@
         <v>-1</v>
       </c>
       <c r="B843" t="s">
-        <v>841</v>
+        <v>840</v>
       </c>
       <c r="C843" t="s">
-        <v>1763</v>
+        <v>1762</v>
       </c>
       <c r="D843">
         <v>-1</v>
@@ -17774,10 +17780,10 @@
         <v>-1</v>
       </c>
       <c r="B844" t="s">
-        <v>842</v>
+        <v>841</v>
       </c>
       <c r="C844" t="s">
-        <v>1764</v>
+        <v>1763</v>
       </c>
       <c r="D844">
         <v>-1</v>
@@ -17788,10 +17794,10 @@
         <v>-1</v>
       </c>
       <c r="B845" t="s">
-        <v>843</v>
+        <v>842</v>
       </c>
       <c r="C845" t="s">
-        <v>1765</v>
+        <v>1764</v>
       </c>
       <c r="D845">
         <v>-1</v>
@@ -17802,10 +17808,10 @@
         <v>-1</v>
       </c>
       <c r="B846" t="s">
-        <v>844</v>
+        <v>843</v>
       </c>
       <c r="C846" t="s">
-        <v>1766</v>
+        <v>1765</v>
       </c>
       <c r="D846">
         <v>-1</v>
@@ -17816,10 +17822,10 @@
         <v>-1</v>
       </c>
       <c r="B847" t="s">
-        <v>845</v>
+        <v>844</v>
       </c>
       <c r="C847" t="s">
-        <v>1767</v>
+        <v>1766</v>
       </c>
       <c r="D847">
         <v>-1</v>
@@ -17830,10 +17836,10 @@
         <v>-1</v>
       </c>
       <c r="B848" t="s">
-        <v>846</v>
+        <v>845</v>
       </c>
       <c r="C848" t="s">
-        <v>1768</v>
+        <v>1767</v>
       </c>
       <c r="D848">
         <v>-1</v>
@@ -17844,10 +17850,10 @@
         <v>-1</v>
       </c>
       <c r="B849" t="s">
-        <v>847</v>
+        <v>846</v>
       </c>
       <c r="C849" t="s">
-        <v>1769</v>
+        <v>1768</v>
       </c>
       <c r="D849">
         <v>-1</v>
@@ -17858,10 +17864,10 @@
         <v>-1</v>
       </c>
       <c r="B850" t="s">
-        <v>848</v>
+        <v>847</v>
       </c>
       <c r="C850" t="s">
-        <v>1770</v>
+        <v>1769</v>
       </c>
       <c r="D850">
         <v>-1</v>
@@ -17872,10 +17878,10 @@
         <v>-1</v>
       </c>
       <c r="B851" t="s">
-        <v>849</v>
+        <v>848</v>
       </c>
       <c r="C851" t="s">
-        <v>1771</v>
+        <v>1770</v>
       </c>
       <c r="D851">
         <v>-1</v>
@@ -17886,10 +17892,10 @@
         <v>-1</v>
       </c>
       <c r="B852" t="s">
-        <v>850</v>
+        <v>849</v>
       </c>
       <c r="C852" t="s">
-        <v>1772</v>
+        <v>1771</v>
       </c>
       <c r="D852">
         <v>-1</v>
@@ -17897,16 +17903,16 @@
     </row>
     <row r="853" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A853">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B853" t="s">
-        <v>851</v>
+        <v>850</v>
       </c>
       <c r="C853" t="s">
-        <v>1773</v>
+        <v>1772</v>
       </c>
       <c r="D853">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="854" spans="1:4" x14ac:dyDescent="0.25">
@@ -17914,24 +17920,24 @@
         <v>1</v>
       </c>
       <c r="B854" t="s">
-        <v>852</v>
+        <v>851</v>
       </c>
       <c r="C854" t="s">
-        <v>1774</v>
+        <v>1773</v>
       </c>
       <c r="D854">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="855" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A855">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B855" t="s">
-        <v>853</v>
+        <v>852</v>
       </c>
       <c r="C855" t="s">
-        <v>1775</v>
+        <v>1774</v>
       </c>
       <c r="D855">
         <v>-1</v>
@@ -17942,10 +17948,10 @@
         <v>-1</v>
       </c>
       <c r="B856" t="s">
-        <v>854</v>
+        <v>853</v>
       </c>
       <c r="C856" t="s">
-        <v>1776</v>
+        <v>1775</v>
       </c>
       <c r="D856">
         <v>-1</v>
@@ -17956,10 +17962,10 @@
         <v>-1</v>
       </c>
       <c r="B857" t="s">
-        <v>855</v>
+        <v>854</v>
       </c>
       <c r="C857" t="s">
-        <v>1777</v>
+        <v>1776</v>
       </c>
       <c r="D857">
         <v>-1</v>
@@ -17970,10 +17976,10 @@
         <v>-1</v>
       </c>
       <c r="B858" t="s">
-        <v>856</v>
+        <v>855</v>
       </c>
       <c r="C858" t="s">
-        <v>1778</v>
+        <v>1777</v>
       </c>
       <c r="D858">
         <v>-1</v>
@@ -17984,10 +17990,10 @@
         <v>-1</v>
       </c>
       <c r="B859" t="s">
-        <v>857</v>
+        <v>856</v>
       </c>
       <c r="C859" t="s">
-        <v>1779</v>
+        <v>1778</v>
       </c>
       <c r="D859">
         <v>-1</v>
@@ -17995,13 +18001,13 @@
     </row>
     <row r="860" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A860">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B860" t="s">
-        <v>858</v>
+        <v>857</v>
       </c>
       <c r="C860" t="s">
-        <v>1780</v>
+        <v>1779</v>
       </c>
       <c r="D860">
         <v>-1</v>
@@ -18009,13 +18015,13 @@
     </row>
     <row r="861" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A861">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B861" t="s">
-        <v>859</v>
+        <v>858</v>
       </c>
       <c r="C861" t="s">
-        <v>1781</v>
+        <v>1780</v>
       </c>
       <c r="D861">
         <v>-1</v>
@@ -18026,10 +18032,10 @@
         <v>-1</v>
       </c>
       <c r="B862" t="s">
-        <v>860</v>
+        <v>859</v>
       </c>
       <c r="C862" t="s">
-        <v>1782</v>
+        <v>1781</v>
       </c>
       <c r="D862">
         <v>-1</v>
@@ -18037,13 +18043,13 @@
     </row>
     <row r="863" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A863">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B863" t="s">
-        <v>861</v>
+        <v>860</v>
       </c>
       <c r="C863" t="s">
-        <v>1783</v>
+        <v>1782</v>
       </c>
       <c r="D863">
         <v>-1</v>
@@ -18051,13 +18057,13 @@
     </row>
     <row r="864" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A864">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B864" t="s">
-        <v>862</v>
+        <v>861</v>
       </c>
       <c r="C864" t="s">
-        <v>1784</v>
+        <v>1783</v>
       </c>
       <c r="D864">
         <v>-1</v>
@@ -18068,10 +18074,10 @@
         <v>-1</v>
       </c>
       <c r="B865" t="s">
-        <v>863</v>
+        <v>862</v>
       </c>
       <c r="C865" t="s">
-        <v>1785</v>
+        <v>1784</v>
       </c>
       <c r="D865">
         <v>-1</v>
@@ -18082,10 +18088,10 @@
         <v>-1</v>
       </c>
       <c r="B866" t="s">
-        <v>864</v>
+        <v>863</v>
       </c>
       <c r="C866" t="s">
-        <v>1786</v>
+        <v>1785</v>
       </c>
       <c r="D866">
         <v>-1</v>
@@ -18096,10 +18102,10 @@
         <v>-1</v>
       </c>
       <c r="B867" t="s">
-        <v>865</v>
+        <v>864</v>
       </c>
       <c r="C867" t="s">
-        <v>1787</v>
+        <v>1786</v>
       </c>
       <c r="D867">
         <v>-1</v>
@@ -18110,10 +18116,10 @@
         <v>-1</v>
       </c>
       <c r="B868" t="s">
-        <v>866</v>
+        <v>865</v>
       </c>
       <c r="C868" t="s">
-        <v>1788</v>
+        <v>1787</v>
       </c>
       <c r="D868">
         <v>-1</v>
@@ -18124,10 +18130,10 @@
         <v>-1</v>
       </c>
       <c r="B869" t="s">
-        <v>867</v>
+        <v>866</v>
       </c>
       <c r="C869" t="s">
-        <v>1789</v>
+        <v>1788</v>
       </c>
       <c r="D869">
         <v>-1</v>
@@ -18138,10 +18144,10 @@
         <v>-1</v>
       </c>
       <c r="B870" t="s">
-        <v>868</v>
+        <v>867</v>
       </c>
       <c r="C870" t="s">
-        <v>1790</v>
+        <v>1789</v>
       </c>
       <c r="D870">
         <v>-1</v>
@@ -18152,10 +18158,10 @@
         <v>-1</v>
       </c>
       <c r="B871" t="s">
-        <v>869</v>
+        <v>868</v>
       </c>
       <c r="C871" t="s">
-        <v>1221</v>
+        <v>1790</v>
       </c>
       <c r="D871">
         <v>-1</v>
@@ -18166,10 +18172,10 @@
         <v>-1</v>
       </c>
       <c r="B872" t="s">
-        <v>870</v>
+        <v>869</v>
       </c>
       <c r="C872" t="s">
-        <v>1791</v>
+        <v>1221</v>
       </c>
       <c r="D872">
         <v>-1</v>
@@ -18180,10 +18186,10 @@
         <v>-1</v>
       </c>
       <c r="B873" t="s">
-        <v>871</v>
+        <v>870</v>
       </c>
       <c r="C873" t="s">
-        <v>1792</v>
+        <v>1791</v>
       </c>
       <c r="D873">
         <v>-1</v>
@@ -18194,10 +18200,10 @@
         <v>-1</v>
       </c>
       <c r="B874" t="s">
-        <v>872</v>
+        <v>871</v>
       </c>
       <c r="C874" t="s">
-        <v>1793</v>
+        <v>1792</v>
       </c>
       <c r="D874">
         <v>-1</v>
@@ -18208,10 +18214,10 @@
         <v>-1</v>
       </c>
       <c r="B875" t="s">
-        <v>873</v>
+        <v>872</v>
       </c>
       <c r="C875" t="s">
-        <v>1794</v>
+        <v>1793</v>
       </c>
       <c r="D875">
         <v>-1</v>
@@ -18222,10 +18228,10 @@
         <v>-1</v>
       </c>
       <c r="B876" t="s">
-        <v>874</v>
+        <v>873</v>
       </c>
       <c r="C876" t="s">
-        <v>1795</v>
+        <v>1794</v>
       </c>
       <c r="D876">
         <v>-1</v>
@@ -18236,10 +18242,10 @@
         <v>-1</v>
       </c>
       <c r="B877" t="s">
-        <v>875</v>
+        <v>874</v>
       </c>
       <c r="C877" t="s">
-        <v>1796</v>
+        <v>1795</v>
       </c>
       <c r="D877">
         <v>-1</v>
@@ -18250,10 +18256,10 @@
         <v>-1</v>
       </c>
       <c r="B878" t="s">
-        <v>876</v>
+        <v>875</v>
       </c>
       <c r="C878" t="s">
-        <v>1797</v>
+        <v>1796</v>
       </c>
       <c r="D878">
         <v>-1</v>
@@ -18264,10 +18270,10 @@
         <v>-1</v>
       </c>
       <c r="B879" t="s">
-        <v>877</v>
+        <v>876</v>
       </c>
       <c r="C879" t="s">
-        <v>1798</v>
+        <v>1797</v>
       </c>
       <c r="D879">
         <v>-1</v>
@@ -18278,10 +18284,10 @@
         <v>-1</v>
       </c>
       <c r="B880" t="s">
-        <v>878</v>
+        <v>877</v>
       </c>
       <c r="C880" t="s">
-        <v>1799</v>
+        <v>1798</v>
       </c>
       <c r="D880">
         <v>-1</v>
@@ -18292,10 +18298,10 @@
         <v>-1</v>
       </c>
       <c r="B881" t="s">
-        <v>879</v>
+        <v>878</v>
       </c>
       <c r="C881" t="s">
-        <v>1800</v>
+        <v>1799</v>
       </c>
       <c r="D881">
         <v>-1</v>
@@ -18306,10 +18312,10 @@
         <v>-1</v>
       </c>
       <c r="B882" t="s">
-        <v>880</v>
+        <v>879</v>
       </c>
       <c r="C882" t="s">
-        <v>1801</v>
+        <v>1800</v>
       </c>
       <c r="D882">
         <v>-1</v>
@@ -18320,10 +18326,10 @@
         <v>-1</v>
       </c>
       <c r="B883" t="s">
-        <v>881</v>
+        <v>880</v>
       </c>
       <c r="C883" t="s">
-        <v>1802</v>
+        <v>1801</v>
       </c>
       <c r="D883">
         <v>-1</v>
@@ -18334,10 +18340,10 @@
         <v>-1</v>
       </c>
       <c r="B884" t="s">
-        <v>882</v>
+        <v>881</v>
       </c>
       <c r="C884" t="s">
-        <v>1803</v>
+        <v>1802</v>
       </c>
       <c r="D884">
         <v>-1</v>
@@ -18348,10 +18354,10 @@
         <v>-1</v>
       </c>
       <c r="B885" t="s">
-        <v>883</v>
+        <v>882</v>
       </c>
       <c r="C885" t="s">
-        <v>1804</v>
+        <v>1803</v>
       </c>
       <c r="D885">
         <v>-1</v>
@@ -18362,10 +18368,10 @@
         <v>-1</v>
       </c>
       <c r="B886" t="s">
-        <v>884</v>
+        <v>883</v>
       </c>
       <c r="C886" t="s">
-        <v>1805</v>
+        <v>1804</v>
       </c>
       <c r="D886">
         <v>-1</v>
@@ -18376,10 +18382,10 @@
         <v>-1</v>
       </c>
       <c r="B887" t="s">
-        <v>885</v>
+        <v>884</v>
       </c>
       <c r="C887" t="s">
-        <v>1806</v>
+        <v>1805</v>
       </c>
       <c r="D887">
         <v>-1</v>
@@ -18390,10 +18396,10 @@
         <v>-1</v>
       </c>
       <c r="B888" t="s">
-        <v>886</v>
+        <v>885</v>
       </c>
       <c r="C888" t="s">
-        <v>1807</v>
+        <v>1806</v>
       </c>
       <c r="D888">
         <v>-1</v>
@@ -18404,10 +18410,10 @@
         <v>-1</v>
       </c>
       <c r="B889" t="s">
-        <v>887</v>
+        <v>886</v>
       </c>
       <c r="C889" t="s">
-        <v>1808</v>
+        <v>1807</v>
       </c>
       <c r="D889">
         <v>-1</v>
@@ -18418,10 +18424,10 @@
         <v>-1</v>
       </c>
       <c r="B890" t="s">
-        <v>888</v>
+        <v>887</v>
       </c>
       <c r="C890" t="s">
-        <v>1809</v>
+        <v>1808</v>
       </c>
       <c r="D890">
         <v>-1</v>
@@ -18432,10 +18438,10 @@
         <v>-1</v>
       </c>
       <c r="B891" t="s">
-        <v>889</v>
+        <v>888</v>
       </c>
       <c r="C891" t="s">
-        <v>1810</v>
+        <v>1809</v>
       </c>
       <c r="D891">
         <v>-1</v>
@@ -18443,16 +18449,16 @@
     </row>
     <row r="892" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A892">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B892" t="s">
-        <v>890</v>
+        <v>889</v>
       </c>
       <c r="C892" t="s">
-        <v>1811</v>
+        <v>1810</v>
       </c>
       <c r="D892">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="893" spans="1:4" x14ac:dyDescent="0.25">
@@ -18460,24 +18466,24 @@
         <v>1</v>
       </c>
       <c r="B893" t="s">
-        <v>891</v>
+        <v>890</v>
       </c>
       <c r="C893" t="s">
-        <v>1812</v>
+        <v>1811</v>
       </c>
       <c r="D893">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="894" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A894">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B894" t="s">
-        <v>892</v>
+        <v>891</v>
       </c>
       <c r="C894" t="s">
-        <v>1813</v>
+        <v>1812</v>
       </c>
       <c r="D894">
         <v>-1</v>
@@ -18488,10 +18494,10 @@
         <v>-1</v>
       </c>
       <c r="B895" t="s">
-        <v>893</v>
+        <v>892</v>
       </c>
       <c r="C895" t="s">
-        <v>1814</v>
+        <v>1813</v>
       </c>
       <c r="D895">
         <v>-1</v>
@@ -18502,10 +18508,10 @@
         <v>-1</v>
       </c>
       <c r="B896" t="s">
-        <v>894</v>
+        <v>893</v>
       </c>
       <c r="C896" t="s">
-        <v>1815</v>
+        <v>1814</v>
       </c>
       <c r="D896">
         <v>-1</v>
@@ -18516,10 +18522,10 @@
         <v>-1</v>
       </c>
       <c r="B897" t="s">
-        <v>895</v>
+        <v>894</v>
       </c>
       <c r="C897" t="s">
-        <v>1816</v>
+        <v>1815</v>
       </c>
       <c r="D897">
         <v>-1</v>
@@ -18530,13 +18536,13 @@
         <v>-1</v>
       </c>
       <c r="B898" t="s">
-        <v>896</v>
+        <v>895</v>
       </c>
       <c r="C898" t="s">
-        <v>1817</v>
+        <v>1816</v>
       </c>
       <c r="D898">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="899" spans="1:4" x14ac:dyDescent="0.25">
@@ -18544,24 +18550,24 @@
         <v>-1</v>
       </c>
       <c r="B899" t="s">
-        <v>897</v>
+        <v>896</v>
       </c>
       <c r="C899" t="s">
-        <v>1818</v>
+        <v>1817</v>
       </c>
       <c r="D899">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="900" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A900">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B900" t="s">
-        <v>898</v>
+        <v>897</v>
       </c>
       <c r="C900" t="s">
-        <v>1819</v>
+        <v>1818</v>
       </c>
       <c r="D900">
         <v>-1</v>
@@ -18569,13 +18575,13 @@
     </row>
     <row r="901" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A901">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B901" t="s">
-        <v>899</v>
+        <v>898</v>
       </c>
       <c r="C901" t="s">
-        <v>1820</v>
+        <v>1819</v>
       </c>
       <c r="D901">
         <v>-1</v>
@@ -18586,10 +18592,10 @@
         <v>-1</v>
       </c>
       <c r="B902" t="s">
-        <v>900</v>
+        <v>899</v>
       </c>
       <c r="C902" t="s">
-        <v>1821</v>
+        <v>1820</v>
       </c>
       <c r="D902">
         <v>-1</v>
@@ -18600,10 +18606,10 @@
         <v>-1</v>
       </c>
       <c r="B903" t="s">
-        <v>901</v>
+        <v>900</v>
       </c>
       <c r="C903" t="s">
-        <v>1822</v>
+        <v>1821</v>
       </c>
       <c r="D903">
         <v>-1</v>
@@ -18614,10 +18620,10 @@
         <v>-1</v>
       </c>
       <c r="B904" t="s">
-        <v>902</v>
+        <v>901</v>
       </c>
       <c r="C904" t="s">
-        <v>1823</v>
+        <v>1822</v>
       </c>
       <c r="D904">
         <v>-1</v>
@@ -18628,10 +18634,10 @@
         <v>-1</v>
       </c>
       <c r="B905" t="s">
-        <v>903</v>
+        <v>902</v>
       </c>
       <c r="C905" t="s">
-        <v>1824</v>
+        <v>1823</v>
       </c>
       <c r="D905">
         <v>-1</v>
@@ -18642,10 +18648,10 @@
         <v>-1</v>
       </c>
       <c r="B906" t="s">
-        <v>904</v>
+        <v>903</v>
       </c>
       <c r="C906" t="s">
-        <v>1825</v>
+        <v>1824</v>
       </c>
       <c r="D906">
         <v>-1</v>
@@ -18656,10 +18662,10 @@
         <v>-1</v>
       </c>
       <c r="B907" t="s">
-        <v>905</v>
+        <v>904</v>
       </c>
       <c r="C907" t="s">
-        <v>1826</v>
+        <v>1825</v>
       </c>
       <c r="D907">
         <v>-1</v>
@@ -18670,10 +18676,10 @@
         <v>-1</v>
       </c>
       <c r="B908" t="s">
-        <v>906</v>
+        <v>905</v>
       </c>
       <c r="C908" t="s">
-        <v>1827</v>
+        <v>1826</v>
       </c>
       <c r="D908">
         <v>-1</v>
@@ -18681,30 +18687,30 @@
     </row>
     <row r="909" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A909">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B909" t="s">
-        <v>907</v>
+        <v>906</v>
       </c>
       <c r="C909" t="s">
-        <v>1828</v>
+        <v>1827</v>
       </c>
       <c r="D909">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="910" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A910">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B910" t="s">
-        <v>908</v>
+        <v>907</v>
       </c>
       <c r="C910" t="s">
-        <v>1829</v>
+        <v>1828</v>
       </c>
       <c r="D910">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="911" spans="1:4" x14ac:dyDescent="0.25">
@@ -18712,10 +18718,10 @@
         <v>-1</v>
       </c>
       <c r="B911" t="s">
-        <v>909</v>
+        <v>908</v>
       </c>
       <c r="C911" t="s">
-        <v>1830</v>
+        <v>1829</v>
       </c>
       <c r="D911">
         <v>-1</v>
@@ -18723,13 +18729,13 @@
     </row>
     <row r="912" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A912">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B912" t="s">
-        <v>910</v>
+        <v>909</v>
       </c>
       <c r="C912" t="s">
-        <v>1831</v>
+        <v>1830</v>
       </c>
       <c r="D912">
         <v>-1</v>
@@ -18737,13 +18743,13 @@
     </row>
     <row r="913" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A913">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B913" t="s">
-        <v>911</v>
+        <v>910</v>
       </c>
       <c r="C913" t="s">
-        <v>1832</v>
+        <v>1831</v>
       </c>
       <c r="D913">
         <v>-1</v>
@@ -18754,10 +18760,10 @@
         <v>-1</v>
       </c>
       <c r="B914" t="s">
-        <v>912</v>
+        <v>911</v>
       </c>
       <c r="C914" t="s">
-        <v>1833</v>
+        <v>1832</v>
       </c>
       <c r="D914">
         <v>-1</v>
@@ -18765,13 +18771,13 @@
     </row>
     <row r="915" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A915">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B915" t="s">
-        <v>913</v>
+        <v>912</v>
       </c>
       <c r="C915" t="s">
-        <v>1834</v>
+        <v>1833</v>
       </c>
       <c r="D915">
         <v>-1</v>
@@ -18779,13 +18785,13 @@
     </row>
     <row r="916" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A916">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B916" t="s">
-        <v>914</v>
+        <v>913</v>
       </c>
       <c r="C916" t="s">
-        <v>1835</v>
+        <v>1834</v>
       </c>
       <c r="D916">
         <v>-1</v>
@@ -18796,10 +18802,10 @@
         <v>-1</v>
       </c>
       <c r="B917" t="s">
-        <v>915</v>
+        <v>914</v>
       </c>
       <c r="C917" t="s">
-        <v>1836</v>
+        <v>1835</v>
       </c>
       <c r="D917">
         <v>-1</v>
@@ -18810,10 +18816,10 @@
         <v>-1</v>
       </c>
       <c r="B918" t="s">
-        <v>916</v>
+        <v>915</v>
       </c>
       <c r="C918" t="s">
-        <v>1837</v>
+        <v>1836</v>
       </c>
       <c r="D918">
         <v>-1</v>
@@ -18824,10 +18830,10 @@
         <v>-1</v>
       </c>
       <c r="B919" t="s">
-        <v>917</v>
+        <v>916</v>
       </c>
       <c r="C919" t="s">
-        <v>1838</v>
+        <v>1837</v>
       </c>
       <c r="D919">
         <v>-1</v>
@@ -18838,10 +18844,10 @@
         <v>-1</v>
       </c>
       <c r="B920" t="s">
-        <v>918</v>
+        <v>917</v>
       </c>
       <c r="C920" t="s">
-        <v>1839</v>
+        <v>1838</v>
       </c>
       <c r="D920">
         <v>-1</v>
@@ -18852,10 +18858,10 @@
         <v>-1</v>
       </c>
       <c r="B921" t="s">
-        <v>919</v>
+        <v>918</v>
       </c>
       <c r="C921" t="s">
-        <v>1840</v>
+        <v>1839</v>
       </c>
       <c r="D921">
         <v>-1</v>
@@ -18866,10 +18872,10 @@
         <v>-1</v>
       </c>
       <c r="B922" t="s">
-        <v>920</v>
+        <v>919</v>
       </c>
       <c r="C922" t="s">
-        <v>1841</v>
+        <v>1840</v>
       </c>
       <c r="D922">
         <v>-1</v>
@@ -18880,10 +18886,10 @@
         <v>-1</v>
       </c>
       <c r="B923" t="s">
-        <v>921</v>
+        <v>920</v>
       </c>
       <c r="C923" t="s">
-        <v>1842</v>
+        <v>1841</v>
       </c>
       <c r="D923">
         <v>-1</v>
@@ -18894,10 +18900,10 @@
         <v>-1</v>
       </c>
       <c r="B924" t="s">
-        <v>922</v>
+        <v>921</v>
       </c>
       <c r="C924" t="s">
-        <v>1843</v>
+        <v>1842</v>
       </c>
       <c r="D924">
         <v>-1</v>
@@ -18908,10 +18914,10 @@
         <v>-1</v>
       </c>
       <c r="B925" t="s">
-        <v>923</v>
+        <v>922</v>
       </c>
       <c r="C925" t="s">
-        <v>1844</v>
+        <v>1843</v>
       </c>
       <c r="D925">
         <v>-1</v>
@@ -18922,10 +18928,10 @@
         <v>-1</v>
       </c>
       <c r="B926" t="s">
-        <v>924</v>
+        <v>923</v>
       </c>
       <c r="C926" t="s">
-        <v>1845</v>
+        <v>1844</v>
       </c>
       <c r="D926">
         <v>-1</v>
@@ -18936,10 +18942,10 @@
         <v>-1</v>
       </c>
       <c r="B927" t="s">
-        <v>925</v>
+        <v>924</v>
       </c>
       <c r="C927" t="s">
-        <v>1846</v>
+        <v>1845</v>
       </c>
       <c r="D927">
         <v>-1</v>
@@ -18950,10 +18956,10 @@
         <v>-1</v>
       </c>
       <c r="B928" t="s">
-        <v>926</v>
+        <v>925</v>
       </c>
       <c r="C928" t="s">
-        <v>1847</v>
+        <v>1846</v>
       </c>
       <c r="D928">
         <v>-1</v>
@@ -18961,13 +18967,13 @@
     </row>
     <row r="929" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A929">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B929" t="s">
-        <v>927</v>
+        <v>926</v>
       </c>
       <c r="C929" t="s">
-        <v>1848</v>
+        <v>1847</v>
       </c>
       <c r="D929">
         <v>-1</v>
@@ -18975,13 +18981,13 @@
     </row>
     <row r="930" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A930">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B930" t="s">
-        <v>928</v>
+        <v>927</v>
       </c>
       <c r="C930" t="s">
-        <v>1849</v>
+        <v>1848</v>
       </c>
       <c r="D930">
         <v>-1</v>
@@ -18989,16 +18995,16 @@
     </row>
     <row r="931" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A931">
-        <v>1</v>
+        <v>-1</v>
       </c>
       <c r="B931" t="s">
-        <v>929</v>
+        <v>928</v>
       </c>
       <c r="C931" t="s">
-        <v>1850</v>
+        <v>1849</v>
       </c>
       <c r="D931">
-        <v>1</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="932" spans="1:4" x14ac:dyDescent="0.25">
@@ -19006,24 +19012,24 @@
         <v>1</v>
       </c>
       <c r="B932" t="s">
-        <v>930</v>
+        <v>929</v>
       </c>
       <c r="C932" t="s">
-        <v>1851</v>
+        <v>1850</v>
       </c>
       <c r="D932">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="933" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A933">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="B933" t="s">
-        <v>931</v>
+        <v>930</v>
       </c>
       <c r="C933" t="s">
-        <v>1852</v>
+        <v>1851</v>
       </c>
       <c r="D933">
         <v>-1</v>
@@ -19034,10 +19040,10 @@
         <v>-1</v>
       </c>
       <c r="B934" t="s">
-        <v>932</v>
+        <v>931</v>
       </c>
       <c r="C934" t="s">
-        <v>1853</v>
+        <v>1852</v>
       </c>
       <c r="D934">
         <v>-1</v>
@@ -19048,10 +19054,10 @@
         <v>-1</v>
       </c>
       <c r="B935" t="s">
-        <v>933</v>
+        <v>932</v>
       </c>
       <c r="C935" t="s">
-        <v>1854</v>
+        <v>1853</v>
       </c>
       <c r="D935">
         <v>-1</v>
@@ -19062,12 +19068,26 @@
         <v>-1</v>
       </c>
       <c r="B936" t="s">
+        <v>933</v>
+      </c>
+      <c r="C936" t="s">
+        <v>1854</v>
+      </c>
+      <c r="D936">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="937" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A937">
+        <v>-1</v>
+      </c>
+      <c r="B937" t="s">
         <v>934</v>
       </c>
-      <c r="C936" t="s">
+      <c r="C937" t="s">
         <v>1855</v>
       </c>
-      <c r="D936">
+      <c r="D937">
         <v>-1</v>
       </c>
     </row>

</xml_diff>